<commit_message>
Figure updates + file renaming
</commit_message>
<xml_diff>
--- a/1_data/unemployment-inactivity-hiring.xlsx
+++ b/1_data/unemployment-inactivity-hiring.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ugentbe-my.sharepoint.com/personal/louis_lippens_ugent_be/Documents/Postdoc Louis/01_research/10_coauthorship/Liam D'hert/unemployment-inactivity-hiring/1_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="588" documentId="13_ncr:1_{88FE8787-B12A-3242-8DE7-4A6F07BD7DAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D01BAB48-5661-4924-A303-C78B3ABB43E3}"/>
+  <xr:revisionPtr revIDLastSave="589" documentId="13_ncr:1_{88FE8787-B12A-3242-8DE7-4A6F07BD7DAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2219008-13E9-4F97-90AC-450923AF9A4E}"/>
   <bookViews>
-    <workbookView xWindow="-75" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{12CDA854-A7F8-4C8D-9788-EEF2E75C1570}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{12CDA854-A7F8-4C8D-9788-EEF2E75C1570}"/>
   </bookViews>
   <sheets>
     <sheet name="unemployment-inactivity-hiring" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'unemployment-inactivity-hiring'!$A$1:$AC$94</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1040,7 +1043,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{352076CC-07B2-40C2-8B8E-33849CA7CC61}">
   <dimension ref="A1:AC94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="W1" sqref="W1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -9010,6 +9015,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AC94" xr:uid="{352076CC-07B2-40C2-8B8E-33849CA7CC61}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="I95:I1048576">
     <cfRule type="top10" dxfId="3" priority="1" percent="1" bottom="1" rank="5"/>

</xml_diff>